<commit_message>
fix vacc data and small improvements for report
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2021-05-02.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2021-05-02.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="353">
   <si>
     <t xml:space="preserve">Testungen</t>
   </si>
@@ -377,7 +377,7 @@
     <t xml:space="preserve">108 ( 0,1%)</t>
   </si>
   <si>
-    <t xml:space="preserve"> -8,5%</t>
+    <t xml:space="preserve">-8,5%</t>
   </si>
   <si>
     <t xml:space="preserve">60 bis 79 Jahre</t>
@@ -389,7 +389,7 @@
     <t xml:space="preserve">549 ( 3,5%)</t>
   </si>
   <si>
-    <t xml:space="preserve"> -1,4%</t>
+    <t xml:space="preserve">-1,4%</t>
   </si>
   <si>
     <t xml:space="preserve">80 Jahre +</t>
@@ -401,7 +401,7 @@
     <t xml:space="preserve">615 (16,5%)</t>
   </si>
   <si>
-    <t xml:space="preserve"> -5,2%</t>
+    <t xml:space="preserve">-5,2%</t>
   </si>
   <si>
     <t xml:space="preserve">Gesamt</t>
@@ -413,7 +413,7 @@
     <t xml:space="preserve">1272 ( 1,2%)</t>
   </si>
   <si>
-    <t xml:space="preserve"> -3,9%</t>
+    <t xml:space="preserve">-3,9%</t>
   </si>
   <si>
     <t xml:space="preserve">Übersterblichkeit</t>
@@ -425,7 +425,7 @@
     <t xml:space="preserve">-52 (-3,0%)</t>
   </si>
   <si>
-    <t xml:space="preserve">-72,3%</t>
+    <t xml:space="preserve">72,3%</t>
   </si>
   <si>
     <t xml:space="preserve">-592 ( -8,8%)</t>
@@ -434,7 +434,7 @@
     <t xml:space="preserve">-364 (-5,6%)</t>
   </si>
   <si>
-    <t xml:space="preserve">-38,5%</t>
+    <t xml:space="preserve">38,5%</t>
   </si>
   <si>
     <t xml:space="preserve">-534 ( -4,8%)</t>
@@ -443,7 +443,7 @@
     <t xml:space="preserve">-117 (-1,1%)</t>
   </si>
   <si>
-    <t xml:space="preserve">-78,1%</t>
+    <t xml:space="preserve">78,1%</t>
   </si>
   <si>
     <t xml:space="preserve">-1314 ( -6,7%)</t>
@@ -452,7 +452,7 @@
     <t xml:space="preserve">-534 (-2,8%)</t>
   </si>
   <si>
-    <t xml:space="preserve">-59,4%</t>
+    <t xml:space="preserve">59,4%</t>
   </si>
   <si>
     <t xml:space="preserve">Vorwarnzeit</t>
@@ -798,22 +798,46 @@
     <t xml:space="preserve">Geimpfte Personen</t>
   </si>
   <si>
-    <t xml:space="preserve">Stand 4.5.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23860165 (28,7 %)</t>
+    <t xml:space="preserve">Stand 5.5.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anteil_Veraenderung</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">20521685 (24,7 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24546919 (29,5 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4,8 PP</t>
   </si>
   <si>
     <t xml:space="preserve">Nicht vollst. geimpft</t>
   </si>
   <si>
-    <t xml:space="preserve">17088689 (20,5 %)</t>
+    <t xml:space="preserve">14407957 (17,3 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17615335 (21,2 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3,9 PP</t>
   </si>
   <si>
     <t xml:space="preserve">Vollst. geimpft</t>
   </si>
   <si>
-    <t xml:space="preserve">6771476 ( 8,1 %)</t>
+    <t xml:space="preserve">6113728 ( 7,4 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6931584 ( 8,3 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,0 PP</t>
   </si>
   <si>
     <t xml:space="preserve">Impffortschritt</t>
@@ -828,12 +852,18 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t xml:space="preserve">   NA %</t>
+  </si>
+  <si>
     <t xml:space="preserve">3493652</t>
   </si>
   <si>
     <t xml:space="preserve">4637884</t>
   </si>
   <si>
+    <t xml:space="preserve"> 32,8 %</t>
+  </si>
+  <si>
     <t xml:space="preserve">davon in Impfzentren</t>
   </si>
   <si>
@@ -843,6 +873,9 @@
     <t xml:space="preserve">2412430 ( 52 %)</t>
   </si>
   <si>
+    <t xml:space="preserve"> -1,7 %</t>
+  </si>
+  <si>
     <t xml:space="preserve">davon in ärztl. Praxen</t>
   </si>
   <si>
@@ -852,6 +885,9 @@
     <t xml:space="preserve">2225454 ( 48 %)</t>
   </si>
   <si>
+    <t xml:space="preserve">114,3 %</t>
+  </si>
+  <si>
     <t xml:space="preserve">Impfungen Praxen</t>
   </si>
   <si>
@@ -861,100 +897,91 @@
     <t xml:space="preserve">Gesamt vollst.</t>
   </si>
   <si>
-    <t xml:space="preserve">28,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28,2</t>
+    <t xml:space="preserve">29,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,0</t>
   </si>
   <si>
     <t xml:space="preserve"> 7,8</t>
   </si>
   <si>
-    <t xml:space="preserve">29,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29,8</t>
+    <t xml:space="preserve">27,1</t>
   </si>
   <si>
     <t xml:space="preserve">10,0</t>
   </si>
   <si>
-    <t xml:space="preserve">29,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27,6</t>
+    <t xml:space="preserve">26,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31,0</t>
   </si>
   <si>
     <t xml:space="preserve"> 7,9</t>
   </si>
   <si>
-    <t xml:space="preserve">30,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28,1</t>
+    <t xml:space="preserve">28,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33,1</t>
   </si>
   <si>
     <t xml:space="preserve"> 9,0</t>
   </si>
   <si>
-    <t xml:space="preserve">32,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11,8</t>
+    <t xml:space="preserve">26,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,2</t>
   </si>
   <si>
     <t xml:space="preserve">Impfstoffdosen</t>
@@ -966,64 +993,103 @@
     <t xml:space="preserve">Biontech/Pfizer</t>
   </si>
   <si>
-    <t xml:space="preserve">22768239 (74,3 %)</t>
+    <t xml:space="preserve">19465427 (73,1 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23399097 (74,4 %)</t>
   </si>
   <si>
     <t xml:space="preserve">Erstimpfungen</t>
   </si>
   <si>
-    <t xml:space="preserve">16515448</t>
+    <t xml:space="preserve">13756748</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17014901</t>
   </si>
   <si>
     <t xml:space="preserve">Zweitimpfungen</t>
   </si>
   <si>
-    <t xml:space="preserve">6252791</t>
+    <t xml:space="preserve">5708679</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6384196</t>
   </si>
   <si>
     <t xml:space="preserve">geliefert</t>
   </si>
   <si>
-    <t xml:space="preserve">23561043</t>
+    <t xml:space="preserve">23564774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25378274</t>
   </si>
   <si>
     <t xml:space="preserve">Moderna</t>
   </si>
   <si>
-    <t xml:space="preserve">1872526 ( 6,1 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1435533</t>
-  </si>
-  <si>
-    <t xml:space="preserve">436993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2598000</t>
+    <t xml:space="preserve">1507091 ( 5,7 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1932692 ( 6,1 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1134048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1482621</t>
+  </si>
+  <si>
+    <t xml:space="preserve">373043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">450071</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2742000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3118800</t>
   </si>
   <si>
     <t xml:space="preserve">AstraZeneca</t>
   </si>
   <si>
-    <t xml:space="preserve">5975398 (19,5 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5901445</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73953</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6895330</t>
+    <t xml:space="preserve">5661991 (21,3 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6127132 (19,5 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5630437</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6039606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31554</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87526</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6899998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6959998</t>
   </si>
   <si>
     <t xml:space="preserve">Johnson&amp;Johnson</t>
   </si>
   <si>
-    <t xml:space="preserve">7739 ( 0,0 %)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">232800</t>
+    <t xml:space="preserve">452 ( 0,0 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9791 ( 0,0 %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">256800</t>
   </si>
 </sst>
 </file>
@@ -1455,24 +1521,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>262</v>
+        <v>270</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="B2" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="C2" t="s">
-        <v>264</v>
+        <v>272</v>
+      </c>
+      <c r="D2" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="3">
@@ -1480,32 +1552,41 @@
         <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="C3" t="s">
-        <v>266</v>
+        <v>275</v>
+      </c>
+      <c r="D3" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="B4" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="C4" t="s">
-        <v>269</v>
+        <v>279</v>
+      </c>
+      <c r="D4" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="B5" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>283</v>
+      </c>
+      <c r="D5" t="s">
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -1527,13 +1608,13 @@
         <v>152</v>
       </c>
       <c r="B1" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="C1" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="D1" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="E1" t="s">
         <v>156</v>
@@ -1550,10 +1631,10 @@
         <v>2225454</v>
       </c>
       <c r="C2" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="D2" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="E2" t="n">
         <v>133</v>
@@ -1570,10 +1651,10 @@
         <v>280712</v>
       </c>
       <c r="C3" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="D3" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="E3" t="n">
         <v>163</v>
@@ -1590,10 +1671,10 @@
         <v>364493</v>
       </c>
       <c r="C4" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="D4" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
       <c r="E4" t="n">
         <v>132</v>
@@ -1610,10 +1691,10 @@
         <v>91933</v>
       </c>
       <c r="C5" t="s">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="D5" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
       <c r="E5" t="n">
         <v>106</v>
@@ -1630,10 +1711,10 @@
         <v>77876</v>
       </c>
       <c r="C6" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="D6" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="E6" t="n">
         <v>101</v>
@@ -1650,10 +1731,10 @@
         <v>16164</v>
       </c>
       <c r="C7" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="D7" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="E7" t="n">
         <v>123</v>
@@ -1670,10 +1751,10 @@
         <v>41480</v>
       </c>
       <c r="C8" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="D8" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="E8" t="n">
         <v>86</v>
@@ -1690,10 +1771,10 @@
         <v>155826</v>
       </c>
       <c r="C9" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="D9" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E9" t="n">
         <v>139</v>
@@ -1710,10 +1791,10 @@
         <v>60758</v>
       </c>
       <c r="C10" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="D10" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="E10" t="n">
         <v>106</v>
@@ -1730,10 +1811,10 @@
         <v>211481</v>
       </c>
       <c r="C11" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="D11" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="E11" t="n">
         <v>93</v>
@@ -1750,10 +1831,10 @@
         <v>510837</v>
       </c>
       <c r="C12" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="D12" t="s">
-        <v>279</v>
+        <v>305</v>
       </c>
       <c r="E12" t="n">
         <v>148</v>
@@ -1770,10 +1851,10 @@
         <v>102537</v>
       </c>
       <c r="C13" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="D13" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="E13" t="n">
         <v>114</v>
@@ -1790,10 +1871,10 @@
         <v>28266</v>
       </c>
       <c r="C14" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="D14" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="E14" t="n">
         <v>128</v>
@@ -1810,10 +1891,10 @@
         <v>96387</v>
       </c>
       <c r="C15" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="D15" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="E15" t="n">
         <v>179</v>
@@ -1830,10 +1911,10 @@
         <v>56623</v>
       </c>
       <c r="C16" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="D16" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="E16" t="n">
         <v>132</v>
@@ -1850,10 +1931,10 @@
         <v>77368</v>
       </c>
       <c r="C17" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="D17" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="E17" t="n">
         <v>54</v>
@@ -1870,10 +1951,10 @@
         <v>52713</v>
       </c>
       <c r="C18" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="D18" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="E18" t="n">
         <v>209</v>
@@ -1898,122 +1979,167 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="B1" t="s">
-        <v>309</v>
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="B2" t="s">
-        <v>311</v>
+        <v>320</v>
+      </c>
+      <c r="C2" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="B3" t="s">
-        <v>313</v>
+        <v>323</v>
+      </c>
+      <c r="C3" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="B4" t="s">
-        <v>315</v>
+        <v>326</v>
+      </c>
+      <c r="C4" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="B5" t="s">
-        <v>317</v>
+        <v>329</v>
+      </c>
+      <c r="C5" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>318</v>
+        <v>331</v>
       </c>
       <c r="B6" t="s">
-        <v>319</v>
+        <v>332</v>
+      </c>
+      <c r="C6" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="B7" t="s">
-        <v>320</v>
+        <v>334</v>
+      </c>
+      <c r="C7" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="B8" t="s">
-        <v>321</v>
+        <v>336</v>
+      </c>
+      <c r="C8" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="B9" t="s">
-        <v>322</v>
+        <v>338</v>
+      </c>
+      <c r="C9" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>323</v>
+        <v>340</v>
       </c>
       <c r="B10" t="s">
-        <v>324</v>
+        <v>341</v>
+      </c>
+      <c r="C10" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
       <c r="B11" t="s">
-        <v>325</v>
+        <v>343</v>
+      </c>
+      <c r="C11" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="B12" t="s">
-        <v>326</v>
+        <v>345</v>
+      </c>
+      <c r="C12" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="B13" t="s">
-        <v>327</v>
+        <v>347</v>
+      </c>
+      <c r="C13" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>328</v>
+        <v>349</v>
       </c>
       <c r="B14" t="s">
-        <v>329</v>
+        <v>350</v>
+      </c>
+      <c r="C14" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="B15" t="s">
-        <v>330</v>
+        <v>352</v>
+      </c>
+      <c r="C15" t="s">
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3455,7 +3581,13 @@
         <v>254</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>255</v>
+      </c>
+      <c r="D1" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="2">
@@ -3463,29 +3595,51 @@
         <v>30</v>
       </c>
       <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>256</v>
+        <v>258</v>
+      </c>
+      <c r="C3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D3" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B4" t="s">
-        <v>258</v>
+        <v>262</v>
+      </c>
+      <c r="C4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D4" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="B5" t="s">
-        <v>260</v>
+        <v>266</v>
+      </c>
+      <c r="C5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D5" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>